<commit_message>
added generate_RBN, deleted random_initial
</commit_message>
<xml_diff>
--- a/pandas_to_excel.xlsx
+++ b/pandas_to_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,12 +447,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0]</t>
+          <t>[0, 0, 0]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[0, 1, 0, 0, 0]</t>
+          <t>[1, 1, 1]</t>
         </is>
       </c>
     </row>
@@ -462,12 +462,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[0, 1, 0, 0, 0]</t>
+          <t>[1, 1, 1]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[0, 1, 0, 0, 0]</t>
+          <t>[0, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -477,12 +477,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[1, 0, 0, 0, 0]</t>
+          <t>[1, 0, 0]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[0, 1, 1, 0, 0]</t>
+          <t>[1, 1, 1]</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[0, 1, 1, 0, 0]</t>
+          <t>[0, 1, 0]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1, 0]</t>
+          <t>[1, 1, 1]</t>
         </is>
       </c>
     </row>
@@ -507,12 +507,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1, 0]</t>
+          <t>[1, 1, 0]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[0, 1, 0, 0, 0]</t>
+          <t>[1, 1, 0]</t>
         </is>
       </c>
     </row>
@@ -522,12 +522,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[1, 1, 0, 0, 0]</t>
+          <t>[0, 0, 1]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[0, 1, 1, 0, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
     </row>
@@ -537,12 +537,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[0, 0, 1, 0, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
     </row>
@@ -552,372 +552,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[1, 0, 1, 0, 0]</t>
+          <t>[0, 1, 1]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[0, 0, 1, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>[1, 1, 1, 0, 0]</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>[0, 0, 1, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>[1, 0, 0, 1, 0]</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>[0, 1, 1, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>[0, 1, 0, 1, 0]</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>[0, 1, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>[1, 1, 0, 1, 0]</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>[0, 1, 1, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>[0, 0, 1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 1, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>[1, 0, 1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>[0, 0, 1, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>[0, 1, 1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 1, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>[1, 1, 1, 1, 0]</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>[0, 0, 1, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 1]</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>[1, 0, 0, 0, 1]</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>[0, 1, 0, 0, 1]</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>[1, 1, 0, 0, 1]</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>[0, 0, 1, 0, 1]</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 1, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>[1, 0, 1, 0, 1]</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>[0, 1, 1, 0, 1]</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 1, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>[1, 1, 1, 0, 1]</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 1, 1]</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>[1, 0, 0, 1, 1]</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>[0, 1, 0, 1, 1]</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>[1, 1, 0, 1, 1]</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>[0, 0, 1, 1, 1]</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 1, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>[1, 0, 1, 1, 1]</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>[0, 1, 1, 1, 1]</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 1, 0]</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>[1, 1, 1, 1, 1]</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0]</t>
+          <t>[0, 0, 1]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added functionality of fidning networks of 2 point attractors
</commit_message>
<xml_diff>
--- a/pandas_to_excel.xlsx
+++ b/pandas_to_excel.xlsx
@@ -452,7 +452,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[1, 1, 1]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
     </row>
@@ -462,7 +462,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[1, 1, 1]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -482,7 +482,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[1, 1, 1]</t>
+          <t>[0, 0, 1]</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[0, 1, 0]</t>
+          <t>[0, 0, 1]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[1, 1, 1]</t>
+          <t>[1, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -507,12 +507,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[0, 1, 0]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[1, 1, 0]</t>
+          <t>[1, 0, 1]</t>
         </is>
       </c>
     </row>
@@ -522,12 +522,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>[1, 1, 0]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>[0, 0, 1]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>[1, 0, 1]</t>
         </is>
       </c>
     </row>
@@ -537,12 +537,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[1, 0, 1]</t>
+          <t>[0, 1, 1]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[1, 0, 1]</t>
+          <t>[1, 0, 0]</t>
         </is>
       </c>
     </row>
@@ -552,12 +552,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[0, 1, 1]</t>
+          <t>[1, 1, 1]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[0, 0, 1]</t>
+          <t>[0, 0, 0]</t>
         </is>
       </c>
     </row>

</xml_diff>